<commit_message>
test results training on nature ecoli
</commit_message>
<xml_diff>
--- a/indigoData/asm_data.xlsx
+++ b/indigoData/asm_data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="18">
   <si>
     <t>TRM</t>
   </si>
@@ -109,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -123,11 +123,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -135,6 +137,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2104,10 +2108,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -2115,10 +2119,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C2">
@@ -2126,10 +2130,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -2137,10 +2141,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4">
@@ -2148,10 +2152,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C5">
@@ -2159,10 +2163,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -2170,10 +2174,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -2181,10 +2185,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -2192,10 +2196,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C9">
@@ -2203,10 +2207,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10">
@@ -2214,10 +2218,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C11">
@@ -2225,10 +2229,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C12">
@@ -2236,10 +2240,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C13">
@@ -2247,10 +2251,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C14">
@@ -2258,10 +2262,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C15">
@@ -2269,10 +2273,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C16">
@@ -2280,10 +2284,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C17">
@@ -2291,10 +2295,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C18">
@@ -2302,10 +2306,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C19">
@@ -2313,10 +2317,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C20">
@@ -2324,10 +2328,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C21">
@@ -2335,10 +2339,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C22">
@@ -2346,10 +2350,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C23">
@@ -2357,10 +2361,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C24">
@@ -2368,10 +2372,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C25">
@@ -2379,10 +2383,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C26">
@@ -2390,10 +2394,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C27">
@@ -2401,10 +2405,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C28">
@@ -2412,10 +2416,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C29">
@@ -2423,10 +2427,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C30">
@@ -2434,10 +2438,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C31">
@@ -2445,10 +2449,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C32">
@@ -2456,10 +2460,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C33">
@@ -2467,10 +2471,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C34">
@@ -2478,10 +2482,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C35">
@@ -2489,10 +2493,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C36">
@@ -2500,10 +2504,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C37">
@@ -2511,10 +2515,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C38">
@@ -2522,10 +2526,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C39">
@@ -2533,10 +2537,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C40">
@@ -2544,10 +2548,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C41">
@@ -2555,10 +2559,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C42">
@@ -2566,10 +2570,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C43">
@@ -2577,10 +2581,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C44">
@@ -2588,10 +2592,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C45">
@@ -2599,10 +2603,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C46">
@@ -2610,10 +2614,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C47">
@@ -2621,10 +2625,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C48">
@@ -2632,10 +2636,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C49">
@@ -2643,10 +2647,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C50">
@@ -2654,10 +2658,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C51">
@@ -2665,10 +2669,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C52">
@@ -2676,10 +2680,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C53">
@@ -2687,10 +2691,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C54">
@@ -2698,10 +2702,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C55">
@@ -2709,10 +2713,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C56">
@@ -2720,10 +2724,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C57">
@@ -2731,10 +2735,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C58">
@@ -2742,10 +2746,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C59">
@@ -2753,10 +2757,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C60">
@@ -2764,10 +2768,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C61">
@@ -2775,10 +2779,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C62">
@@ -2786,10 +2790,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C63">
@@ -2797,10 +2801,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C64">
@@ -2808,10 +2812,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C65">
@@ -2819,10 +2823,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C66">
@@ -2830,10 +2834,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C67">
@@ -2841,10 +2845,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C68">
@@ -2852,10 +2856,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C69">
@@ -2863,10 +2867,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C70">
@@ -2874,10 +2878,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C71">
@@ -2885,10 +2889,10 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C72">
@@ -2896,10 +2900,10 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C73">
@@ -2907,10 +2911,10 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C74">
@@ -2918,10 +2922,10 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C75">
@@ -2929,10 +2933,10 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C76">
@@ -2940,10 +2944,10 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C77">
@@ -2951,10 +2955,10 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C78">
@@ -2962,10 +2966,10 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C79">
@@ -2973,10 +2977,10 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C80">
@@ -2984,10 +2988,10 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C81">
@@ -2995,10 +2999,10 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C82">
@@ -3006,10 +3010,10 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C83">
@@ -3017,10 +3021,10 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C84">
@@ -3028,10 +3032,10 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C85">
@@ -3039,10 +3043,10 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C86">
@@ -3050,10 +3054,10 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C87">
@@ -3061,10 +3065,10 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C88">
@@ -3072,10 +3076,10 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C89">
@@ -3083,10 +3087,10 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C90">
@@ -3094,10 +3098,10 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C91">
@@ -3105,10 +3109,10 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C92">
@@ -3116,10 +3120,10 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C93">
@@ -3127,10 +3131,10 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C94">
@@ -3138,10 +3142,10 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C95">
@@ -3149,10 +3153,10 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C96">
@@ -3160,10 +3164,10 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C97">
@@ -3171,10 +3175,10 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C98">
@@ -3182,10 +3186,10 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C99">
@@ -3193,10 +3197,10 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C100">
@@ -3204,10 +3208,10 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C101">
@@ -3215,10 +3219,10 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C102">
@@ -3226,10 +3230,10 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C103">
@@ -3237,10 +3241,10 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C104">
@@ -3248,10 +3252,10 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C105">
@@ -3259,10 +3263,10 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C106">
@@ -3270,10 +3274,10 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C107">
@@ -3281,10 +3285,10 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C108">
@@ -3292,10 +3296,10 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C109">
@@ -3303,10 +3307,10 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C110">
@@ -3314,10 +3318,10 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="5" t="s">
+      <c r="A111" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C111">
@@ -3325,10 +3329,10 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="5" t="s">
+      <c r="A112" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C112">
@@ -3336,10 +3340,10 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="5" t="s">
+      <c r="A113" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C113">
@@ -3347,10 +3351,10 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="5" t="s">
+      <c r="A114" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C114">
@@ -3358,10 +3362,10 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="5" t="s">
+      <c r="A115" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B115" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C115">
@@ -3369,10 +3373,10 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B116" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C116">
@@ -3380,10 +3384,10 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="5" t="s">
+      <c r="A117" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C117">
@@ -3391,10 +3395,10 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B118" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C118">
@@ -3402,10 +3406,10 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="5" t="s">
+      <c r="A119" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B119" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C119">
@@ -3413,10 +3417,10 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="5" t="s">
+      <c r="A120" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="B120" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C120">
@@ -3424,10 +3428,10 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C121">
@@ -3435,10 +3439,10 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="5" t="s">
+      <c r="A122" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C122">
@@ -3446,10 +3450,10 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="5" t="s">
+      <c r="A123" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B123" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C123">
@@ -3457,10 +3461,10 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="5" t="s">
+      <c r="A124" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C124">
@@ -3468,10 +3472,10 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="5" t="s">
+      <c r="A125" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C125">
@@ -3479,10 +3483,10 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="5" t="s">
+      <c r="A126" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C126">
@@ -3490,10 +3494,10 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C127">
@@ -3501,10 +3505,10 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="5" t="s">
+      <c r="A128" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B128" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C128">
@@ -3512,10 +3516,10 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="5" t="s">
+      <c r="A129" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="B129" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C129">
@@ -3523,10 +3527,10 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="5" t="s">
+      <c r="A130" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C130">
@@ -3534,10 +3538,10 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="5" t="s">
+      <c r="A131" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C131">
@@ -3545,10 +3549,10 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B132" s="5" t="s">
+      <c r="A132" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C132">
@@ -3556,10 +3560,10 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B133" s="5" t="s">
+      <c r="A133" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C133">
@@ -3567,10 +3571,10 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B134" s="5" t="s">
+      <c r="A134" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C134">
@@ -3578,10 +3582,10 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B135" s="5" t="s">
+      <c r="A135" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C135">
@@ -3589,10 +3593,10 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B136" s="5" t="s">
+      <c r="A136" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C136">
@@ -3600,10 +3604,10 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B137" s="5" t="s">
+      <c r="A137" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C137">
@@ -3611,10 +3615,10 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B138" s="5" t="s">
+      <c r="A138" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C138">
@@ -3622,10 +3626,10 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B139" s="5" t="s">
+      <c r="A139" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C139">
@@ -3633,10 +3637,10 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B140" s="5" t="s">
+      <c r="A140" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C140">
@@ -3644,10 +3648,10 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B141" s="5" t="s">
+      <c r="A141" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C141">
@@ -3655,10 +3659,10 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B142" s="5" t="s">
+      <c r="A142" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B142" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C142">
@@ -3666,10 +3670,10 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B143" s="5" t="s">
+      <c r="A143" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C143">
@@ -3677,10 +3681,10 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B144" s="5" t="s">
+      <c r="A144" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B144" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C144">
@@ -3688,10 +3692,10 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B145" s="5" t="s">
+      <c r="A145" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C145">
@@ -3699,10 +3703,10 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B146" s="5" t="s">
+      <c r="A146" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B146" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C146">
@@ -3710,10 +3714,10 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B147" s="5" t="s">
+      <c r="A147" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C147">
@@ -3721,10 +3725,10 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B148" s="5" t="s">
+      <c r="A148" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B148" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C148">

</xml_diff>